<commit_message>
add Gas-Oil OMG-832 SCAL
</commit_message>
<xml_diff>
--- a/Miscible_flooding/OIL.xlsx
+++ b/Miscible_flooding/OIL.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fractional_flow\Miscible_flooding\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{143086F9-C986-4C8D-AE98-0E224011F328}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0A85B69-E733-44A4-8417-8ABFAD805A6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10245" windowHeight="8985" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SCAL" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="SCAL1" sheetId="5" r:id="rId2"/>
+    <sheet name="SCAL2" sheetId="6" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="22">
   <si>
     <t>SW</t>
   </si>
@@ -90,12 +92,24 @@
   <si>
     <t>Liq Sat</t>
   </si>
+  <si>
+    <t>Sg, frac</t>
+  </si>
+  <si>
+    <t>Kro,frac</t>
+  </si>
+  <si>
+    <t>Krg,frac</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,16 +117,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -120,13 +154,50 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2372,10 +2443,1162 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1FE1CCE-5DFA-4CEF-99E2-A7EA507C3E02}">
+  <dimension ref="A1:C51"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C51"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1.6653299999999999E-16</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>5.8836699999999997E-3</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.90203999999999995</v>
+      </c>
+      <c r="C3" s="2">
+        <v>3.0356600000000001E-7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>1.17673E-2</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.81191199999999997</v>
+      </c>
+      <c r="C4" s="2">
+        <v>3.4344600000000001E-6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>1.7651E-2</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.72913600000000001</v>
+      </c>
+      <c r="C5" s="2">
+        <v>1.41964E-5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>2.3534699999999999E-2</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.653254</v>
+      </c>
+      <c r="C6" s="2">
+        <v>3.8856500000000003E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>2.9418400000000001E-2</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.58382500000000004</v>
+      </c>
+      <c r="C7" s="2">
+        <v>8.4849400000000001E-5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>3.5302E-2</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.52042900000000003</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1.60614E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>4.1185699999999999E-2</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0.46266400000000002</v>
+      </c>
+      <c r="C9" s="2">
+        <v>2.7548399999999999E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>4.7069399999999997E-2</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0.41014600000000001</v>
+      </c>
+      <c r="C10" s="2">
+        <v>4.3961100000000002E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>5.2953100000000003E-2</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0.36251</v>
+      </c>
+      <c r="C11" s="2">
+        <v>6.6390000000000004E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>5.8836699999999999E-2</v>
+      </c>
+      <c r="B12" s="2">
+        <v>0.31940600000000002</v>
+      </c>
+      <c r="C12" s="2">
+        <v>9.5996099999999995E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>6.4720399999999997E-2</v>
+      </c>
+      <c r="B13" s="2">
+        <v>0.280503</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1.3400700000000001E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>7.0604100000000003E-2</v>
+      </c>
+      <c r="B14" s="2">
+        <v>0.24548700000000001</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1.8171400000000001E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>7.6487799999999995E-2</v>
+      </c>
+      <c r="B15" s="2">
+        <v>0.214058</v>
+      </c>
+      <c r="C15" s="2">
+        <v>2.4046699999999998E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>8.2371399999999997E-2</v>
+      </c>
+      <c r="B16" s="2">
+        <v>0.18593399999999999</v>
+      </c>
+      <c r="C16" s="2">
+        <v>3.1167500000000002E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>8.8255100000000003E-2</v>
+      </c>
+      <c r="B17" s="2">
+        <v>0.16084699999999999</v>
+      </c>
+      <c r="C17" s="2">
+        <v>3.9680100000000001E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>9.4138799999999995E-2</v>
+      </c>
+      <c r="B18" s="2">
+        <v>0.138545</v>
+      </c>
+      <c r="C18" s="2">
+        <v>4.9736299999999997E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>0.100022</v>
+      </c>
+      <c r="B19" s="2">
+        <v>0.118787</v>
+      </c>
+      <c r="C19" s="2">
+        <v>6.14929E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>0.105906</v>
+      </c>
+      <c r="B20" s="2">
+        <v>0.101351</v>
+      </c>
+      <c r="C20" s="2">
+        <v>7.5111700000000002E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>0.11179</v>
+      </c>
+      <c r="B21" s="2">
+        <v>8.6025199999999996E-2</v>
+      </c>
+      <c r="C21" s="2">
+        <v>9.0759299999999994E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>0.117673</v>
+      </c>
+      <c r="B22" s="2">
+        <v>7.2612200000000002E-2</v>
+      </c>
+      <c r="C22" s="2">
+        <v>1.0860699999999999E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>0.123557</v>
+      </c>
+      <c r="B23" s="2">
+        <v>6.0927000000000002E-2</v>
+      </c>
+      <c r="C23" s="2">
+        <v>1.28831E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>0.129441</v>
+      </c>
+      <c r="B24" s="2">
+        <v>5.0797000000000002E-2</v>
+      </c>
+      <c r="C24" s="2">
+        <v>1.51612E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>0.135324</v>
+      </c>
+      <c r="B25" s="2">
+        <v>4.20617E-2</v>
+      </c>
+      <c r="C25" s="2">
+        <v>1.7713400000000001E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>0.141208</v>
+      </c>
+      <c r="B26" s="2">
+        <v>3.4571600000000001E-2</v>
+      </c>
+      <c r="C26" s="2">
+        <v>2.05586E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>0.147092</v>
+      </c>
+      <c r="B27" s="2">
+        <v>2.8188700000000001E-2</v>
+      </c>
+      <c r="C27" s="2">
+        <v>2.37161E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>0.152976</v>
+      </c>
+      <c r="B28" s="2">
+        <v>2.27855E-2</v>
+      </c>
+      <c r="C28" s="2">
+        <v>2.7205699999999999E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>0.158859</v>
+      </c>
+      <c r="B29" s="2">
+        <v>1.82445E-2</v>
+      </c>
+      <c r="C29" s="2">
+        <v>3.1047499999999999E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>0.164743</v>
+      </c>
+      <c r="B30" s="2">
+        <v>1.44583E-2</v>
+      </c>
+      <c r="C30" s="2">
+        <v>3.5262000000000002E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>0.170627</v>
+      </c>
+      <c r="B31" s="2">
+        <v>1.1328400000000001E-2</v>
+      </c>
+      <c r="C31" s="2">
+        <v>3.9870000000000003E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>0.17651</v>
+      </c>
+      <c r="B32" s="2">
+        <v>8.7657199999999994E-3</v>
+      </c>
+      <c r="C32" s="2">
+        <v>4.4892899999999999E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>0.182394</v>
+      </c>
+      <c r="B33" s="2">
+        <v>6.6893200000000003E-3</v>
+      </c>
+      <c r="C33" s="2">
+        <v>5.0352300000000003E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>0.188278</v>
+      </c>
+      <c r="B34" s="2">
+        <v>5.0264799999999998E-3</v>
+      </c>
+      <c r="C34" s="2">
+        <v>5.6270199999999999E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>0.194161</v>
+      </c>
+      <c r="B35" s="2">
+        <v>3.7120999999999999E-3</v>
+      </c>
+      <c r="C35" s="2">
+        <v>6.2669000000000002E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>0.200045</v>
+      </c>
+      <c r="B36" s="2">
+        <v>2.6882899999999999E-3</v>
+      </c>
+      <c r="C36" s="2">
+        <v>6.9571300000000003E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <v>0.205929</v>
+      </c>
+      <c r="B37" s="2">
+        <v>1.9039700000000001E-3</v>
+      </c>
+      <c r="C37" s="2">
+        <v>7.7000200000000005E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>0.211812</v>
+      </c>
+      <c r="B38" s="2">
+        <v>1.3144299999999999E-3</v>
+      </c>
+      <c r="C38" s="2">
+        <v>8.4979200000000005E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
+        <v>0.217696</v>
+      </c>
+      <c r="B39" s="2">
+        <v>8.8089799999999997E-4</v>
+      </c>
+      <c r="C39" s="2">
+        <v>9.3531900000000001E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
+        <v>0.22358</v>
+      </c>
+      <c r="B40" s="2">
+        <v>5.7014200000000004E-4</v>
+      </c>
+      <c r="C40" s="2">
+        <v>0.102682</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
+        <v>0.229463</v>
+      </c>
+      <c r="B41" s="2">
+        <v>3.5401299999999997E-4</v>
+      </c>
+      <c r="C41" s="2">
+        <v>0.112455</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
+        <v>0.235347</v>
+      </c>
+      <c r="B42" s="2">
+        <v>2.0904100000000001E-4</v>
+      </c>
+      <c r="C42" s="2">
+        <v>0.122875</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
+        <v>0.241231</v>
+      </c>
+      <c r="B43" s="2">
+        <v>1.1600299999999999E-4</v>
+      </c>
+      <c r="C43" s="2">
+        <v>0.133967</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
+        <v>0.247114</v>
+      </c>
+      <c r="B44" s="2">
+        <v>5.9499000000000001E-5</v>
+      </c>
+      <c r="C44" s="2">
+        <v>0.145756</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="2">
+        <v>0.252998</v>
+      </c>
+      <c r="B45" s="2">
+        <v>2.7528100000000002E-5</v>
+      </c>
+      <c r="C45" s="2">
+        <v>0.15826799999999999</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
+        <v>0.258882</v>
+      </c>
+      <c r="B46" s="2">
+        <v>1.10629E-5</v>
+      </c>
+      <c r="C46" s="2">
+        <v>0.17152899999999999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="2">
+        <v>0.26476499999999997</v>
+      </c>
+      <c r="B47" s="2">
+        <v>3.6250999999999998E-6</v>
+      </c>
+      <c r="C47" s="2">
+        <v>0.18556600000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
+        <v>0.27064899999999997</v>
+      </c>
+      <c r="B48" s="2">
+        <v>8.6025199999999999E-7</v>
+      </c>
+      <c r="C48" s="2">
+        <v>0.200404</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="2">
+        <v>0.27653299999999997</v>
+      </c>
+      <c r="B49" s="2">
+        <v>1.13284E-7</v>
+      </c>
+      <c r="C49" s="2">
+        <v>0.21607100000000001</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="2">
+        <v>0.282416</v>
+      </c>
+      <c r="B50" s="2">
+        <v>3.5401299999999999E-9</v>
+      </c>
+      <c r="C50" s="2">
+        <v>0.232594</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="3">
+        <v>0.2883</v>
+      </c>
+      <c r="B51" s="3">
+        <v>0</v>
+      </c>
+      <c r="C51" s="3">
+        <v>0.2571</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3117CBF1-4156-422E-83DC-02761985CB23}">
+  <dimension ref="A1:C51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2.6781599999999999E-2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.95960000000000001</v>
+      </c>
+      <c r="C3" s="2">
+        <v>2.97495E-5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3.3563299999999997E-2</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.92003299999999999</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1.6828899999999999E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>4.0344900000000003E-2</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.88129900000000005</v>
+      </c>
+      <c r="C5" s="2">
+        <v>4.6374900000000001E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>4.7126500000000002E-2</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.84339900000000001</v>
+      </c>
+      <c r="C6" s="2">
+        <v>9.5198400000000001E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>5.3908200000000003E-2</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.80633100000000002</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1.6630499999999999E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>6.0689800000000002E-2</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.770096</v>
+      </c>
+      <c r="C8" s="2">
+        <v>2.6233599999999999E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>6.7471400000000001E-2</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0.73469399999999996</v>
+      </c>
+      <c r="C9" s="2">
+        <v>3.8567800000000002E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>7.4253100000000002E-2</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0.700125</v>
+      </c>
+      <c r="C10" s="2">
+        <v>5.3852400000000003E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>8.1034700000000001E-2</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0.66638900000000001</v>
+      </c>
+      <c r="C11" s="2">
+        <v>7.2291300000000003E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>8.78163E-2</v>
+      </c>
+      <c r="B12" s="2">
+        <v>0.63348599999999999</v>
+      </c>
+      <c r="C12" s="2">
+        <v>9.4076200000000002E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>9.4598000000000002E-2</v>
+      </c>
+      <c r="B13" s="2">
+        <v>0.60141599999999995</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1.1938799999999999E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>0.10138</v>
+      </c>
+      <c r="B14" s="2">
+        <v>0.57017899999999999</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1.4840000000000001E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>0.10816099999999999</v>
+      </c>
+      <c r="B15" s="2">
+        <v>0.539775</v>
+      </c>
+      <c r="C15" s="2">
+        <v>1.8127500000000001E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>0.114943</v>
+      </c>
+      <c r="B16" s="2">
+        <v>0.51020399999999999</v>
+      </c>
+      <c r="C16" s="2">
+        <v>2.1817199999999998E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>0.121724</v>
+      </c>
+      <c r="B17" s="2">
+        <v>0.48146600000000001</v>
+      </c>
+      <c r="C17" s="2">
+        <v>2.59244E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>0.12850600000000001</v>
+      </c>
+      <c r="B18" s="2">
+        <v>0.45356099999999999</v>
+      </c>
+      <c r="C18" s="2">
+        <v>3.0463500000000001E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>0.13528799999999999</v>
+      </c>
+      <c r="B19" s="2">
+        <v>0.42648900000000001</v>
+      </c>
+      <c r="C19" s="2">
+        <v>3.5448800000000003E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>0.142069</v>
+      </c>
+      <c r="B20" s="2">
+        <v>0.40024999999999999</v>
+      </c>
+      <c r="C20" s="2">
+        <v>4.0894100000000003E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>0.14885100000000001</v>
+      </c>
+      <c r="B21" s="2">
+        <v>0.37484400000000001</v>
+      </c>
+      <c r="C21" s="2">
+        <v>4.6812699999999999E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>0.15563299999999999</v>
+      </c>
+      <c r="B22" s="2">
+        <v>0.350271</v>
+      </c>
+      <c r="C22" s="2">
+        <v>5.3217500000000001E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>0.162414</v>
+      </c>
+      <c r="B23" s="2">
+        <v>0.32653100000000002</v>
+      </c>
+      <c r="C23" s="2">
+        <v>6.0121300000000003E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>0.16919600000000001</v>
+      </c>
+      <c r="B24" s="2">
+        <v>0.30362299999999998</v>
+      </c>
+      <c r="C24" s="2">
+        <v>6.7536200000000005E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>0.175978</v>
+      </c>
+      <c r="B25" s="2">
+        <v>0.28154899999999999</v>
+      </c>
+      <c r="C25" s="2">
+        <v>7.5474399999999997E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>0.182759</v>
+      </c>
+      <c r="B26" s="2">
+        <v>0.26030799999999998</v>
+      </c>
+      <c r="C26" s="2">
+        <v>8.3947499999999994E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>0.18954099999999999</v>
+      </c>
+      <c r="B27" s="2">
+        <v>0.2399</v>
+      </c>
+      <c r="C27" s="2">
+        <v>9.29672E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>0.196322</v>
+      </c>
+      <c r="B28" s="2">
+        <v>0.22032499999999999</v>
+      </c>
+      <c r="C28" s="2">
+        <v>0.102545</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>0.20310400000000001</v>
+      </c>
+      <c r="B29" s="2">
+        <v>0.20158300000000001</v>
+      </c>
+      <c r="C29" s="2">
+        <v>0.112691</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>0.20988599999999999</v>
+      </c>
+      <c r="B30" s="2">
+        <v>0.183673</v>
+      </c>
+      <c r="C30" s="2">
+        <v>0.123417</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>0.216667</v>
+      </c>
+      <c r="B31" s="2">
+        <v>0.166597</v>
+      </c>
+      <c r="C31" s="2">
+        <v>0.13473299999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>0.22344900000000001</v>
+      </c>
+      <c r="B32" s="2">
+        <v>0.15035399999999999</v>
+      </c>
+      <c r="C32" s="2">
+        <v>0.14665</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>0.23023099999999999</v>
+      </c>
+      <c r="B33" s="2">
+        <v>0.13494400000000001</v>
+      </c>
+      <c r="C33" s="2">
+        <v>0.15917799999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>0.237012</v>
+      </c>
+      <c r="B34" s="2">
+        <v>0.120367</v>
+      </c>
+      <c r="C34" s="2">
+        <v>0.17232800000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>0.24379400000000001</v>
+      </c>
+      <c r="B35" s="2">
+        <v>0.10662199999999999</v>
+      </c>
+      <c r="C35" s="2">
+        <v>0.186108</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>0.25057600000000002</v>
+      </c>
+      <c r="B36" s="2">
+        <v>9.3711000000000003E-2</v>
+      </c>
+      <c r="C36" s="2">
+        <v>0.20052900000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <v>0.257357</v>
+      </c>
+      <c r="B37" s="2">
+        <v>8.1632700000000002E-2</v>
+      </c>
+      <c r="C37" s="2">
+        <v>0.21560099999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>0.26413900000000001</v>
+      </c>
+      <c r="B38" s="2">
+        <v>7.03873E-2</v>
+      </c>
+      <c r="C38" s="2">
+        <v>0.23133200000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
+        <v>0.27091999999999999</v>
+      </c>
+      <c r="B39" s="2">
+        <v>5.9975000000000001E-2</v>
+      </c>
+      <c r="C39" s="2">
+        <v>0.24773300000000001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
+        <v>0.277702</v>
+      </c>
+      <c r="B40" s="2">
+        <v>5.0395700000000002E-2</v>
+      </c>
+      <c r="C40" s="2">
+        <v>0.26481300000000002</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
+        <v>0.28448400000000001</v>
+      </c>
+      <c r="B41" s="2">
+        <v>4.16493E-2</v>
+      </c>
+      <c r="C41" s="2">
+        <v>0.28258</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
+        <v>0.291265</v>
+      </c>
+      <c r="B42" s="2">
+        <v>3.3735899999999999E-2</v>
+      </c>
+      <c r="C42" s="2">
+        <v>0.30104399999999998</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
+        <v>0.29804700000000001</v>
+      </c>
+      <c r="B43" s="2">
+        <v>2.6655600000000002E-2</v>
+      </c>
+      <c r="C43" s="2">
+        <v>0.32021300000000003</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
+        <v>0.30482900000000002</v>
+      </c>
+      <c r="B44" s="2">
+        <v>2.0408200000000001E-2</v>
+      </c>
+      <c r="C44" s="2">
+        <v>0.34009699999999998</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="2">
+        <v>0.31161</v>
+      </c>
+      <c r="B45" s="2">
+        <v>1.49938E-2</v>
+      </c>
+      <c r="C45" s="2">
+        <v>0.36070400000000002</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
+        <v>0.31839200000000001</v>
+      </c>
+      <c r="B46" s="2">
+        <v>1.0412299999999999E-2</v>
+      </c>
+      <c r="C46" s="2">
+        <v>0.38204199999999999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="2">
+        <v>0.32517299999999999</v>
+      </c>
+      <c r="B47" s="2">
+        <v>6.6638899999999996E-3</v>
+      </c>
+      <c r="C47" s="2">
+        <v>0.40412100000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
+        <v>0.331955</v>
+      </c>
+      <c r="B48" s="2">
+        <v>3.74844E-3</v>
+      </c>
+      <c r="C48" s="2">
+        <v>0.42694700000000002</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="2">
+        <v>0.33873700000000001</v>
+      </c>
+      <c r="B49" s="2">
+        <v>1.6659699999999999E-3</v>
+      </c>
+      <c r="C49" s="2">
+        <v>0.45053100000000001</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="2">
+        <v>0.34551799999999999</v>
+      </c>
+      <c r="B50" s="2">
+        <v>4.1649299999999998E-4</v>
+      </c>
+      <c r="C50" s="2">
+        <v>0.474879</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="3">
+        <v>0.3523</v>
+      </c>
+      <c r="B51" s="3">
+        <v>0</v>
+      </c>
+      <c r="C51" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B37F92AF-96BC-479D-9DF0-ABE2F5BF203D}">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" activeCellId="1" sqref="B5:B19 D5:D19"/>
     </sheetView>
   </sheetViews>

</xml_diff>